<commit_message>
Created spreadsheet for Gerudo Valley
</commit_message>
<xml_diff>
--- a/Notes to Feedrates.xlsx
+++ b/Notes to Feedrates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conta\Documents\Instructables and Projects\Ender 3 Music\Musical Marlin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B142C2F-03E1-4798-812B-8ACE4722AD60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7208D541-00BC-4A10-8AD7-F2AF82371EE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -305,7 +305,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,12 +389,6 @@
       <color theme="0" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -833,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>